<commit_message>
192 process timings added.
git-svn-id: svn://136.177.114.72/svn_GW/phast3/trunk@9724 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/src/phast/yeti2.xlsx
+++ b/src/phast/yeti2.xlsx
@@ -337,6 +337,9 @@
                 <c:pt idx="7">
                   <c:v>18.855498631482909</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.527853659234255</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -519,15 +522,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="399796768"/>
-        <c:axId val="399802208"/>
+        <c:axId val="86190528"/>
+        <c:axId val="86187808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="399796768"/>
+        <c:axId val="86190528"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="128"/>
+          <c:max val="256"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -624,16 +627,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399802208"/>
+        <c:crossAx val="86187808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="399802208"/>
+        <c:axId val="86187808"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="128"/>
+          <c:max val="256"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -744,7 +747,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399796768"/>
+        <c:crossAx val="86190528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1053,6 +1056,9 @@
                 <c:pt idx="5">
                   <c:v>5.7975530446581036</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5445014945865925</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1130,6 +1136,9 @@
                 <c:pt idx="5">
                   <c:v>8.2579625216738215</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.2235487821693027</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1207,6 +1216,9 @@
                 <c:pt idx="5">
                   <c:v>15.745775730984473</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.971255647823451</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1220,15 +1232,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="399802752"/>
-        <c:axId val="399801120"/>
+        <c:axId val="86191616"/>
+        <c:axId val="31396128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="399802752"/>
+        <c:axId val="86191616"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="128"/>
+          <c:max val="256"/>
           <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1326,16 +1338,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399801120"/>
+        <c:crossAx val="31396128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="399801120"/>
+        <c:axId val="31396128"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="32"/>
+          <c:max val="48"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1446,7 +1458,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399802752"/>
+        <c:crossAx val="86191616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1550,9 +1562,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Easy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1567,10 +1576,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$B$10</c:f>
+              <c:f>Sheet1!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -1588,16 +1597,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$5:$O$10</c:f>
+              <c:f>Sheet1!$O$5:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>281.30306469920538</c:v>
                 </c:pt>
@@ -1615,6 +1627,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>48.52099886492622</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.363223609534614</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1624,9 +1639,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Medium</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1641,10 +1653,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$B$31</c:f>
+              <c:f>Sheet1!$B$26:$B$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -1662,16 +1674,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$26:$O$31</c:f>
+              <c:f>Sheet1!$O$26:$O$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1010.9114642451758</c:v>
                 </c:pt>
@@ -1689,6 +1704,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>122.41657207718501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>139.94665153234959</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1698,9 +1716,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>Hard</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1715,10 +1730,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$37:$B$42</c:f>
+              <c:f>Sheet1!$B$37:$B$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>4</c:v>
                 </c:pt>
@@ -1736,16 +1751,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$37:$O$42</c:f>
+              <c:f>Sheet1!$O$37:$O$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>10261.080590238364</c:v>
                 </c:pt>
@@ -1763,6 +1781,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>651.67196367763904</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>540.87514188422244</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1777,15 +1798,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="399805472"/>
-        <c:axId val="399808192"/>
+        <c:axId val="31396672"/>
+        <c:axId val="31397216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="399805472"/>
+        <c:axId val="31396672"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
-          <c:max val="128"/>
+          <c:max val="256"/>
           <c:min val="4"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1897,12 +1918,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399808192"/>
+        <c:crossAx val="31397216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="399808192"/>
+        <c:axId val="31397216"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2018,7 +2039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="399805472"/>
+        <c:crossAx val="31396672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4129,8 +4150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4263,7 +4284,7 @@
         <v>349.19</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" ref="F4:F10" si="0">E4+D4</f>
+        <f t="shared" ref="F4:F11" si="0">E4+D4</f>
         <v>1641</v>
       </c>
       <c r="G4" s="2">
@@ -4281,7 +4302,7 @@
         <v>4606.6100000000006</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" ref="K4:K10" si="1">H4+G4+E4+D4+C4</f>
+        <f t="shared" ref="K4:K11" si="1">H4+G4+E4+D4+C4</f>
         <v>6251.8300000000008</v>
       </c>
       <c r="L4" s="2">
@@ -4293,7 +4314,7 @@
         <v>1.7496944607856968</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O10" si="2">J4/8.81</f>
+        <f t="shared" ref="O4:O11" si="2">J4/8.81</f>
         <v>522.8842224744609</v>
       </c>
     </row>
@@ -4325,11 +4346,11 @@
         <v>635.74</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" ref="I5:I10" si="3">G5</f>
+        <f t="shared" ref="I5:I11" si="3">G5</f>
         <v>1842.54</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" ref="J5:J10" si="4">H5+G5</f>
+        <f t="shared" ref="J5:J11" si="4">H5+G5</f>
         <v>2478.2799999999997</v>
       </c>
       <c r="K5" s="2">
@@ -4337,11 +4358,11 @@
         <v>3511.37</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" ref="L5:L10" si="5">$I$3/I5</f>
+        <f t="shared" ref="L5:L11" si="5">$I$3/I5</f>
         <v>3.3537996461406538</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" ref="M5:M10" si="6">$J$3/J5</f>
+        <f t="shared" ref="M5:M11" si="6">$J$3/J5</f>
         <v>3.2523201575286089</v>
       </c>
       <c r="N5" s="2">
@@ -4401,7 +4422,7 @@
         <v>5.7740431110442501</v>
       </c>
       <c r="N6" s="2">
-        <f t="shared" ref="N6:N10" si="8">$J$5/J6</f>
+        <f t="shared" ref="N6:N11" si="8">$J$5/J6</f>
         <v>1.7753612287149065</v>
       </c>
       <c r="O6">
@@ -4641,18 +4662,53 @@
       <c r="B11">
         <v>192</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="C11" s="2">
+        <v>1.01</v>
+      </c>
+      <c r="D11" s="2">
+        <v>51.97</v>
+      </c>
+      <c r="E11" s="2">
+        <v>625.05999999999995</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>677.03</v>
+      </c>
+      <c r="G11" s="2">
+        <v>264.16000000000003</v>
+      </c>
+      <c r="H11" s="2">
+        <v>435.03</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="3"/>
+        <v>264.16000000000003</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="4"/>
+        <v>699.19</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="1"/>
+        <v>1377.23</v>
+      </c>
+      <c r="L11" s="2">
+        <f t="shared" si="5"/>
+        <v>23.393057238037553</v>
+      </c>
+      <c r="M11" s="2">
+        <f t="shared" si="6"/>
+        <v>11.527853659234255</v>
+      </c>
+      <c r="N11" s="2">
+        <f t="shared" si="8"/>
+        <v>3.5445014945865925</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>79.363223609534614</v>
+      </c>
     </row>
     <row r="13" spans="1:17" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -5101,7 +5157,7 @@
         <v>349.21</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" ref="F25:F31" si="16">E25+D25</f>
+        <f t="shared" ref="F25:F32" si="16">E25+D25</f>
         <v>1665.82</v>
       </c>
       <c r="G25" s="2">
@@ -5119,19 +5175,19 @@
         <v>34700.57</v>
       </c>
       <c r="K25" s="2">
-        <f t="shared" ref="K25:K31" si="17">H25+G25+E25+D25+C25</f>
+        <f t="shared" ref="K25:K32" si="17">H25+G25+E25+D25+C25</f>
         <v>36366.39</v>
       </c>
       <c r="L25" s="2">
-        <f t="shared" ref="L25:L31" si="18">$I$24/I25</f>
+        <f t="shared" ref="L25:L32" si="18">$I$24/I25</f>
         <v>1.9199655781096527</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" ref="M25:M31" si="19">$J$24/J25</f>
+        <f t="shared" ref="M25:M32" si="19">$J$24/J25</f>
         <v>1.9147864141712945</v>
       </c>
       <c r="O25">
-        <f t="shared" ref="O25:O31" si="20">J25/8.81</f>
+        <f t="shared" ref="O25:O32" si="20">J25/8.81</f>
         <v>3938.7707150964811</v>
       </c>
     </row>
@@ -5163,11 +5219,11 @@
         <v>660.72</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" ref="I26:I31" si="21">G26</f>
+        <f t="shared" ref="I26:I32" si="21">G26</f>
         <v>8245.41</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" ref="J26:J31" si="22">H26+G26</f>
+        <f t="shared" ref="J26:J32" si="22">H26+G26</f>
         <v>8906.1299999999992</v>
       </c>
       <c r="K26" s="2">
@@ -5239,7 +5295,7 @@
         <v>12.855179378834398</v>
       </c>
       <c r="N27" s="2">
-        <f t="shared" ref="N27:N31" si="24">$J$26/J27</f>
+        <f t="shared" ref="N27:N32" si="24">$J$26/J27</f>
         <v>1.7230989790410298</v>
       </c>
       <c r="O27">
@@ -5479,18 +5535,53 @@
       <c r="B32">
         <v>192</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+      <c r="C32" s="2">
+        <v>1.41</v>
+      </c>
+      <c r="D32" s="2">
+        <v>48.12</v>
+      </c>
+      <c r="E32" s="2">
+        <v>639.77</v>
+      </c>
+      <c r="F32" s="2">
+        <f t="shared" si="16"/>
+        <v>687.89</v>
+      </c>
+      <c r="G32" s="2">
+        <v>788.14</v>
+      </c>
+      <c r="H32" s="2">
+        <v>444.79</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="21"/>
+        <v>788.14</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="22"/>
+        <v>1232.93</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="17"/>
+        <v>1922.23</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="18"/>
+        <v>82.886999771614185</v>
+      </c>
+      <c r="M32" s="2">
+        <f t="shared" si="19"/>
+        <v>53.891283365641186</v>
+      </c>
+      <c r="N32" s="2">
+        <f t="shared" si="24"/>
+        <v>7.2235487821693027</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="20"/>
+        <v>139.94665153234959</v>
+      </c>
     </row>
     <row r="34" spans="1:15" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
@@ -5583,7 +5674,7 @@
         <v>56.7</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" ref="F37:F42" si="25">E37+D37</f>
+        <f t="shared" ref="F37:F43" si="25">E37+D37</f>
         <v>1074.83</v>
       </c>
       <c r="G37" s="2">
@@ -5593,15 +5684,15 @@
         <v>814.54</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" ref="I37:I42" si="26">G37</f>
+        <f t="shared" ref="I37:I43" si="26">G37</f>
         <v>89585.58</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" ref="J37:J42" si="27">H37+G37</f>
+        <f t="shared" ref="J37:J43" si="27">H37+G37</f>
         <v>90400.12</v>
       </c>
       <c r="K37" s="2">
-        <f t="shared" ref="K37:K42" si="28">H37+G37+E37+D37+C37</f>
+        <f t="shared" ref="K37:K43" si="28">H37+G37+E37+D37+C37</f>
         <v>91479.8</v>
       </c>
       <c r="L37" s="2"/>
@@ -5657,11 +5748,11 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2">
-        <f t="shared" ref="N38:N42" si="30">$J$37/J38</f>
+        <f t="shared" ref="N38:N43" si="30">$J$37/J38</f>
         <v>1.8442353543120267</v>
       </c>
       <c r="O38">
-        <f t="shared" ref="O38:O42" si="31">J38/8.81</f>
+        <f t="shared" ref="O38:O43" si="31">J38/8.81</f>
         <v>5563.8671963677634</v>
       </c>
     </row>
@@ -5873,27 +5964,56 @@
       <c r="B43">
         <v>192</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
+      <c r="C43" s="2">
+        <v>1.27</v>
+      </c>
+      <c r="D43" s="2">
+        <v>41.54</v>
+      </c>
+      <c r="E43" s="2">
+        <v>666.06</v>
+      </c>
+      <c r="F43" s="2">
+        <f t="shared" si="25"/>
+        <v>707.59999999999991</v>
+      </c>
+      <c r="G43" s="2">
+        <v>4365.29</v>
+      </c>
+      <c r="H43" s="2">
+        <v>399.82</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="26"/>
+        <v>4365.29</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="27"/>
+        <v>4765.1099999999997</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="28"/>
+        <v>5473.9800000000005</v>
+      </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+      <c r="N43" s="2">
+        <f t="shared" si="30"/>
+        <v>18.971255647823451</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="31"/>
+        <v>540.87514188422244</v>
+      </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="M45">
-        <f>1/14</f>
-        <v>7.1428571428571425E-2</v>
-      </c>
-      <c r="N45">
-        <f>1760/128</f>
-        <v>13.75</v>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="H46">
+        <f>1760/192</f>
+        <v>9.1666666666666661</v>
+      </c>
+      <c r="I46">
+        <f>1/H46</f>
+        <v>0.1090909090909091</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Some changes to solution.
git-svn-id: svn://136.177.114.72/svn_GW/phast3/trunk@10044 1feff8c3-07ed-0310-ac33-dd36852eb9cd
</commit_message>
<xml_diff>
--- a/src/phast/yeti2.xlsx
+++ b/src/phast/yeti2.xlsx
@@ -217,7 +217,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -522,11 +521,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86190528"/>
-        <c:axId val="86187808"/>
+        <c:axId val="1926955632"/>
+        <c:axId val="1926953456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86190528"/>
+        <c:axId val="1926955632"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -560,7 +559,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -627,12 +625,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86187808"/>
+        <c:crossAx val="1926953456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86187808"/>
+        <c:axId val="1926953456"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -680,7 +678,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -747,7 +744,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86190528"/>
+        <c:crossAx val="1926955632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -761,7 +758,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1232,11 +1228,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86191616"/>
-        <c:axId val="31396128"/>
+        <c:axId val="1926957264"/>
+        <c:axId val="1926948016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86191616"/>
+        <c:axId val="1926957264"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1338,12 +1334,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31396128"/>
+        <c:crossAx val="1926948016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31396128"/>
+        <c:axId val="1926948016"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1458,7 +1454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86191616"/>
+        <c:crossAx val="1926957264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1798,11 +1794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="31396672"/>
-        <c:axId val="31397216"/>
+        <c:axId val="1926949104"/>
+        <c:axId val="1926945840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="31396672"/>
+        <c:axId val="1926949104"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -1918,12 +1914,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31397216"/>
+        <c:crossAx val="1926945840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31397216"/>
+        <c:axId val="1926945840"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2039,7 +2035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31396672"/>
+        <c:crossAx val="1926949104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4151,7 +4147,7 @@
   <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+      <selection activeCell="I46" sqref="G46:I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6004,16 +6000,6 @@
       <c r="O43">
         <f t="shared" si="31"/>
         <v>540.87514188422244</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H46">
-        <f>1760/192</f>
-        <v>9.1666666666666661</v>
-      </c>
-      <c r="I46">
-        <f>1/H46</f>
-        <v>0.1090909090909091</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>